<commit_message>
add export excel payment orphan  v1.5.0
</commit_message>
<xml_diff>
--- a/public/sample/orphans.xlsx
+++ b/public/sample/orphans.xlsx
@@ -746,7 +746,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1067,8 +1087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,6 +1102,7 @@
     <col min="9" max="9" width="21.42578125" customWidth="1"/>
     <col min="10" max="10" width="18.28515625" style="2" customWidth="1"/>
     <col min="11" max="11" width="21.42578125" customWidth="1"/>
+    <col min="18" max="18" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
@@ -2576,9 +2597,12 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="I1:I993"/>
   <sortState ref="A2:X1035">
-    <sortCondition sortBy="cellColor" ref="R2:R1035" dxfId="1"/>
+    <sortCondition sortBy="cellColor" ref="R2:R1035" dxfId="3"/>
   </sortState>
   <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R1:R1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>